<commit_message>
file updates from rmi sep 20
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\template_state\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3349944-4AD5-42BA-9375-9DE11110A9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358573D1-7B9E-4091-AAB9-BE175631EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="1470" windowWidth="15450" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15660" yWindow="1890" windowWidth="13065" windowHeight="14850" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="337">
   <si>
     <t>About</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>Tables 5a, 6, 7a, and 9a</t>
+  </si>
+  <si>
+    <t>For states, we set industry values to zero because we already forecast using the AEO 2020 and 2021 data in the script which accounts for covid</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,6 +1638,11 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -28691,7 +28699,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28748,8 +28756,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <f>Calculations!D28</f>
-        <v>1.2770833518757527</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>